<commit_message>
Update exel BOM file
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12203308\Documents\GitHub\Soldering_station_2023\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3450E25D-F7B7-452A-B38B-2D3BD73EF7F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7C1C4A-399F-4BAB-B55E-805510402AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B58B2E48-1E34-4D42-99CC-8624F77FC9E2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="69">
   <si>
     <t>x3</t>
   </si>
@@ -237,6 +237,15 @@
   </si>
   <si>
     <t>Adafruit</t>
+  </si>
+  <si>
+    <t>IEC filtered connector Male Schurter, 6A, 250 VAC, Panel mounting, 2 poles</t>
+  </si>
+  <si>
+    <t>Profile VTLB-wire 3G 0,75mm², white, 2 meter</t>
+  </si>
+  <si>
+    <t>Encoder knob</t>
   </si>
 </sst>
 </file>
@@ -362,8 +371,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4A9B52FE-E9A8-4374-A5AB-E53472D2FF86}" name="Tabel5" displayName="Tabel5" ref="A31:B51" totalsRowShown="0">
-  <autoFilter ref="A31:B51" xr:uid="{4A9B52FE-E9A8-4374-A5AB-E53472D2FF86}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4A9B52FE-E9A8-4374-A5AB-E53472D2FF86}" name="Tabel5" displayName="Tabel5" ref="A31:B54" totalsRowShown="0">
+  <autoFilter ref="A31:B54" xr:uid="{4A9B52FE-E9A8-4374-A5AB-E53472D2FF86}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{C0086D0D-353F-411C-A69E-1ED7F93FE319}" name="Diverse"/>
     <tableColumn id="2" xr3:uid="{A714AF19-38E1-4B65-9B76-38283987E7FE}" name=" "/>
@@ -669,15 +678,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B91787DF-E5D1-43B8-8964-495F5AD54446}">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="68.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1220,6 +1229,36 @@
       </c>
       <c r="C51" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>